<commit_message>
Complete Common Lisp implementation, with home-rolled player schema validator.
</commit_message>
<xml_diff>
--- a/_general_/language-stats.xlsx
+++ b/_general_/language-stats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="33">
   <si>
     <t>Language</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Released</t>
+  </si>
+  <si>
+    <t>Lisp</t>
   </si>
 </sst>
 </file>
@@ -175,10 +178,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H16" totalsRowShown="0">
-  <autoFilter ref="A1:H16"/>
-  <sortState ref="A2:H16">
-    <sortCondition ref="F1:F16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H17" totalsRowShown="0">
+  <autoFilter ref="A1:H17"/>
+  <sortState ref="A2:H17">
+    <sortCondition ref="F1:F17"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="Language"/>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,7 +555,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -561,39 +564,39 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>2012</v>
+        <v>1958</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4">
-        <v>36214</v>
+        <v>15199</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5">
-        <v>54720</v>
+        <v>36214</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
@@ -604,103 +607,103 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>2009</v>
+        <v>2015</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F6">
-        <v>55735</v>
+        <v>54720</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>1990</v>
+        <v>2009</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7">
-        <v>74361</v>
+        <v>55735</v>
       </c>
       <c r="G7" t="s">
         <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8">
-        <v>100031</v>
+        <v>74361</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>2009</v>
+        <v>1993</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9">
-        <v>293883</v>
+        <v>100031</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H9" t="s">
         <v>27</v>
@@ -708,7 +711,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -717,16 +720,16 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F10">
-        <v>336986</v>
+        <v>293883</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H10" t="s">
         <v>27</v>
@@ -734,7 +737,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -743,50 +746,50 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>1969</v>
+        <v>2012</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>887188</v>
+        <v>336986</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>1995</v>
+        <v>1969</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F12">
-        <v>1440412</v>
+        <v>887188</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -795,16 +798,16 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
       <c r="F13">
-        <v>1608244</v>
+        <v>1440412</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H13" t="s">
         <v>27</v>
@@ -812,7 +815,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -821,16 +824,16 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>1989</v>
+        <v>1994</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
       <c r="F14">
-        <v>2509487</v>
+        <v>1608244</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14" t="s">
         <v>27</v>
@@ -838,22 +841,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1996</v>
+        <v>1989</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
       <c r="F15">
-        <v>4480236</v>
+        <v>2509487</v>
       </c>
       <c r="G15" t="s">
         <v>25</v>
@@ -864,27 +867,53 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1996</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>4480236</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
         <v>1</v>
       </c>
-      <c r="D16">
+      <c r="D17">
         <v>1995</v>
       </c>
-      <c r="E16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16">
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17">
         <v>5168516</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>24</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H17" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>